<commit_message>
Participant List and Methods section updated
</commit_message>
<xml_diff>
--- a/Experimental_scripts/Instructions_grids/REPSWITCH_List.xlsx
+++ b/Experimental_scripts/Instructions_grids/REPSWITCH_List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\Experimental_scripts\Instructions_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A532F0CC-1B39-400F-B594-B749BFD6AD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D16206-49C2-4166-818C-16E08A984202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
   <si>
     <t>Participant</t>
   </si>
@@ -171,12 +171,6 @@
     <t>C02</t>
   </si>
   <si>
-    <t>SpanishAoA</t>
-  </si>
-  <si>
-    <t>BEST</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -354,9 +348,6 @@
     <t>Speaks very fast. Short durations.</t>
   </si>
   <si>
-    <t>Long durations</t>
-  </si>
-  <si>
     <t>Angelika Botero Montaña</t>
   </si>
   <si>
@@ -372,15 +363,6 @@
     <t>Patricia García Arenzana</t>
   </si>
   <si>
-    <t>Some RTs are close to 1200-1500ms</t>
-  </si>
-  <si>
-    <t>RTs are relatively slow. Mostly between 1000-1400ms.</t>
-  </si>
-  <si>
-    <t>Relatively slow RTs -- between 1000 and 1500ms; some even close to 2sec. Long durations as well.</t>
-  </si>
-  <si>
     <t>Leire Varela Aranguren</t>
   </si>
   <si>
@@ -409,6 +391,27 @@
   </si>
   <si>
     <t>Has a cut on her right index. No issue in typing. Took off the bandage. Can do the caja.</t>
+  </si>
+  <si>
+    <t>Supertecleador</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>RTs Speak are relatively slow. Mostly between 1000-1400ms.</t>
+  </si>
+  <si>
+    <t>Some RTs Speak are close to 1200-1500ms</t>
+  </si>
+  <si>
+    <t>Long durations Speak</t>
+  </si>
+  <si>
+    <t>Relatively slow RTs Speak -- between 1000 and 1500ms; some even close to 2sec. Long durations as well.</t>
   </si>
 </sst>
 </file>
@@ -1063,9 +1066,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O50" totalsRowShown="0">
-  <autoFilter ref="A1:O50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:N50" totalsRowShown="0">
+  <autoFilter ref="A1:N50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
     <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID"/>
@@ -1077,8 +1080,7 @@
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
     <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento"/>
     <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{7D4D4D5D-E25F-4CB3-8EE9-5A89F5D57012}" name="SpanishAoA"/>
-    <tableColumn id="11" xr3:uid="{F2E1F23C-70DF-440E-B763-D813108EF947}" name="BEST"/>
+    <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador"/>
     <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed"/>
     <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy"/>
   </tableColumns>
@@ -1087,9 +1089,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1127,7 +1129,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1233,7 +1235,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1375,7 +1377,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1415,10 +1417,10 @@
         <v>29</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>30</v>
@@ -1447,7 +1449,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="6">
         <v>9028</v>
@@ -1462,7 +1464,7 @@
         <v>36624</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -1506,7 +1508,7 @@
         <v>37810</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H3" s="8">
         <v>2</v>
@@ -1541,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,14 +1559,15 @@
     <col min="9" max="9" width="31.88671875" customWidth="1"/>
     <col min="10" max="10" width="13.44140625" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" style="18" customWidth="1"/>
-    <col min="12" max="13" width="10.5546875" customWidth="1"/>
-    <col min="14" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1590,28 +1593,25 @@
         <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L1" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="M1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1641,12 +1641,19 @@
         <v>36910</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2">
+        <v>38.72</v>
+      </c>
+      <c r="N2">
+        <v>98.84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1657,7 +1664,7 @@
         <v>11777</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -1676,12 +1683,19 @@
         <v>36978</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3">
+        <v>30.76</v>
+      </c>
+      <c r="N3">
+        <v>98.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1711,12 +1725,19 @@
         <v>36484</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L4" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="N4">
+        <v>95.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1746,12 +1767,19 @@
         <v>36631</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5">
+        <v>43.32</v>
+      </c>
+      <c r="N5">
+        <v>95.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1777,18 +1805,25 @@
         <v>45246</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6" s="11">
         <v>33073</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6">
+        <v>35.6</v>
+      </c>
+      <c r="N6">
+        <v>93.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1808,29 +1843,36 @@
         <v>3</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H7" s="3">
         <v>45246</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J7" s="11">
         <v>38338</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>119</v>
+      </c>
+      <c r="M7">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="N7">
+        <v>89.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1">
         <v>11082</v>
@@ -1845,27 +1887,36 @@
         <v>4</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H8" s="13">
         <v>45250</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J8" s="15">
         <v>37166</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M8">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="N8">
+        <v>89.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1">
         <v>11000</v>
@@ -1892,15 +1943,24 @@
         <v>37264</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L9" t="s">
+        <v>119</v>
+      </c>
+      <c r="M9">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="N9">
+        <v>93.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>11893</v>
@@ -1921,21 +1981,30 @@
         <v>45252</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J10" s="15">
         <v>37200</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="L10" t="s">
+        <v>120</v>
+      </c>
+      <c r="M10">
+        <v>38.6</v>
+      </c>
+      <c r="N10">
+        <v>91.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1">
         <v>10439</v>
@@ -1950,27 +2019,36 @@
         <v>1</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H11" s="13">
         <v>45253</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J11" s="15">
         <v>36893</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L11" t="s">
+        <v>119</v>
+      </c>
+      <c r="M11">
+        <v>32.6</v>
+      </c>
+      <c r="N11">
+        <v>91.14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1">
         <v>11570</v>
@@ -1985,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H12" s="13">
         <v>45257</v>
@@ -1994,15 +2072,24 @@
         <v>37880</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L12" t="s">
+        <v>119</v>
+      </c>
+      <c r="M12">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="N12">
+        <v>98.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1">
         <v>9754</v>
@@ -2023,21 +2110,30 @@
         <v>45257</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J13" s="15">
         <v>37460</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L13" t="s">
+        <v>119</v>
+      </c>
+      <c r="M13">
+        <v>45.88</v>
+      </c>
+      <c r="N13">
+        <v>95.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" s="1">
         <v>10344</v>
@@ -2061,15 +2157,24 @@
         <v>37504</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M14">
+        <v>40.32</v>
+      </c>
+      <c r="N14">
+        <v>93.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1">
         <v>11614</v>
@@ -2084,7 +2189,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H15" s="13">
         <v>45258</v>
@@ -2093,18 +2198,27 @@
         <v>38214</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="T15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="L15" t="s">
+        <v>119</v>
+      </c>
+      <c r="M15">
+        <v>34.04</v>
+      </c>
+      <c r="N15">
+        <v>95.1</v>
+      </c>
+      <c r="S15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
         <v>11782</v>
@@ -2119,7 +2233,7 @@
         <v>4</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H16" s="13">
         <v>45258</v>
@@ -2128,15 +2242,24 @@
         <v>37691</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L16" t="s">
+        <v>119</v>
+      </c>
+      <c r="M16">
+        <v>39.520000000000003</v>
+      </c>
+      <c r="N16">
+        <v>94.88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1">
         <v>11481</v>
@@ -2157,21 +2280,30 @@
         <v>45259</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J17" s="15">
         <v>34028</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="L17" t="s">
+        <v>120</v>
+      </c>
+      <c r="M17">
+        <v>40.68</v>
+      </c>
+      <c r="N17">
+        <v>93.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1">
         <v>11438</v>
@@ -2192,21 +2324,30 @@
         <v>45260</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J18" s="11">
         <v>38244</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L18" t="s">
+        <v>119</v>
+      </c>
+      <c r="M18">
+        <v>44.4</v>
+      </c>
+      <c r="N18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="14">
         <v>2293</v>
@@ -2221,27 +2362,36 @@
         <v>1</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H19" s="13">
         <v>45260</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J19" s="15">
         <v>32903</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L19" t="s">
+        <v>119</v>
+      </c>
+      <c r="M19">
+        <v>35.08</v>
+      </c>
+      <c r="N19">
+        <v>96.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2">
         <v>9818</v>
@@ -2256,27 +2406,36 @@
         <v>2</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H20" s="13">
         <v>45260</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J20" s="15">
         <v>37433</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L20" t="s">
+        <v>119</v>
+      </c>
+      <c r="M20">
+        <v>32.72</v>
+      </c>
+      <c r="N20">
+        <v>81.86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2">
         <v>10983</v>
@@ -2300,15 +2459,24 @@
         <v>37936</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L21" t="s">
+        <v>119</v>
+      </c>
+      <c r="M21">
+        <v>38.159999999999997</v>
+      </c>
+      <c r="N21">
+        <v>97.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2">
         <v>11478</v>
@@ -2329,21 +2497,30 @@
         <v>45261</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J22" s="15">
         <v>34393</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="L22" t="s">
+        <v>120</v>
+      </c>
+      <c r="M22">
+        <v>55.64</v>
+      </c>
+      <c r="N22">
+        <v>97.48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1">
         <v>10464</v>
@@ -2358,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H23" s="13">
         <v>45261</v>
@@ -2367,15 +2544,24 @@
         <v>35659</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M23">
+        <v>52.28</v>
+      </c>
+      <c r="N23">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1">
         <v>10637</v>
@@ -2390,30 +2576,36 @@
         <v>4</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H24" s="13">
         <v>45261</v>
       </c>
       <c r="I24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J24" s="15">
         <v>37869</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="M24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="L24" t="s">
+        <v>119</v>
+      </c>
+      <c r="M24">
+        <v>34.72</v>
+      </c>
+      <c r="N24">
+        <v>90.66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1">
         <v>10443</v>
@@ -2434,24 +2626,33 @@
         <v>45261</v>
       </c>
       <c r="I25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J25" s="15">
         <v>37670</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="T25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L25" t="s">
+        <v>120</v>
+      </c>
+      <c r="M25">
+        <v>50.16</v>
+      </c>
+      <c r="N25">
+        <v>97.14</v>
+      </c>
+      <c r="S25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="14">
         <v>11512</v>
@@ -2475,15 +2676,24 @@
         <v>37838</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L26" t="s">
+        <v>119</v>
+      </c>
+      <c r="M26">
+        <v>34.4</v>
+      </c>
+      <c r="N26">
+        <v>95.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2">
         <v>11124</v>
@@ -2498,7 +2708,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H27" s="13">
         <v>45264</v>
@@ -2507,15 +2717,24 @@
         <v>37040</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="L27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M27">
+        <v>40.72</v>
+      </c>
+      <c r="N27">
+        <v>93.08</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2">
         <v>11600</v>
@@ -2530,27 +2749,36 @@
         <v>2</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H28" s="13">
         <v>45264</v>
       </c>
       <c r="I28" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="J28" s="15">
         <v>38142</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L28" t="s">
+        <v>119</v>
+      </c>
+      <c r="M28">
+        <v>41.68</v>
+      </c>
+      <c r="N28">
+        <v>89.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2">
         <v>3061</v>
@@ -2571,21 +2799,30 @@
         <v>45264</v>
       </c>
       <c r="I29" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="J29" s="15">
         <v>33365</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L29" t="s">
+        <v>119</v>
+      </c>
+      <c r="M29">
+        <v>33.6</v>
+      </c>
+      <c r="N29">
+        <v>87.76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="2">
         <v>11527</v>
@@ -2606,21 +2843,30 @@
         <v>45265</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J30" s="15">
         <v>37810</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L30" t="s">
+        <v>119</v>
+      </c>
+      <c r="M30">
+        <v>43.68</v>
+      </c>
+      <c r="N30">
+        <v>88.68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2">
         <v>2317</v>
@@ -2635,27 +2881,36 @@
         <v>3</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H31" s="13">
         <v>45265</v>
       </c>
       <c r="I31" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J31" s="15">
         <v>33146</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L31" t="s">
+        <v>120</v>
+      </c>
+      <c r="M31">
+        <v>50</v>
+      </c>
+      <c r="N31">
+        <v>95.12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" s="2">
         <v>8175</v>
@@ -2670,7 +2925,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H32" s="13">
         <v>45265</v>
@@ -2679,15 +2934,24 @@
         <v>32922</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L32" t="s">
+        <v>119</v>
+      </c>
+      <c r="M32">
+        <v>43.4</v>
+      </c>
+      <c r="N32">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" s="2">
         <v>1697</v>
@@ -2711,15 +2975,24 @@
         <v>32661</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L33" t="s">
+        <v>119</v>
+      </c>
+      <c r="M33">
+        <v>55.92</v>
+      </c>
+      <c r="N33">
+        <v>92.66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1">
         <v>9039</v>
@@ -2743,15 +3016,24 @@
         <v>35705</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="L34" t="s">
+        <v>120</v>
+      </c>
+      <c r="M34">
+        <v>43.32</v>
+      </c>
+      <c r="N34">
+        <v>95.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" s="2">
         <v>10010</v>
@@ -2766,27 +3048,27 @@
         <v>1</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H35" s="3">
         <v>45272</v>
       </c>
       <c r="I35" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="J35" s="15">
         <v>37475</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="2">
         <v>10415</v>
@@ -2801,7 +3083,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H36" s="3">
         <v>45272</v>
@@ -2810,15 +3092,15 @@
         <v>37515</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" s="2">
         <v>6729</v>
@@ -2842,15 +3124,24 @@
         <v>34059</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="L37" t="s">
+        <v>119</v>
+      </c>
+      <c r="M37">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="N37">
+        <v>98.38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="2">
         <v>11066</v>
@@ -2871,21 +3162,30 @@
         <v>45273</v>
       </c>
       <c r="I38" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J38" s="15">
         <v>37152</v>
       </c>
       <c r="K38" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L38" t="s">
+        <v>119</v>
+      </c>
+      <c r="M38">
+        <v>40.159999999999997</v>
+      </c>
+      <c r="N38">
+        <v>90.36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" s="1">
         <v>9245</v>
@@ -2900,27 +3200,36 @@
         <v>3</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H39" s="13">
         <v>45273</v>
       </c>
       <c r="I39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J39" s="15">
         <v>36607</v>
       </c>
       <c r="K39" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="L39" t="s">
+        <v>119</v>
+      </c>
+      <c r="M39">
+        <v>38.68</v>
+      </c>
+      <c r="N39">
+        <v>95.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C40" s="1">
         <v>11067</v>
@@ -2935,7 +3244,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H40" s="13">
         <v>45273</v>
@@ -2944,15 +3253,24 @@
         <v>35101</v>
       </c>
       <c r="K40" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="L40" t="s">
+        <v>120</v>
+      </c>
+      <c r="M40">
+        <v>66.52</v>
+      </c>
+      <c r="N40">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C41" s="1">
         <v>8819</v>
@@ -2976,15 +3294,15 @@
         <v>35856</v>
       </c>
       <c r="K41" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" s="14">
         <v>6210</v>
@@ -3008,15 +3326,24 @@
         <v>35934</v>
       </c>
       <c r="K42" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="L42" t="s">
+        <v>119</v>
+      </c>
+      <c r="M42">
+        <v>53.68</v>
+      </c>
+      <c r="N42">
+        <v>90.04</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C43" s="2">
         <v>10275</v>
@@ -3031,27 +3358,27 @@
         <v>1</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H43" s="13">
         <v>45307</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J43" s="15">
         <v>33061</v>
       </c>
       <c r="K43" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C44" s="1">
         <v>6835</v>
@@ -3066,27 +3393,27 @@
         <v>2</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H44" s="13">
         <v>45309</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J44" s="15">
         <v>33718</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C45" s="14">
         <v>10964</v>
@@ -3110,15 +3437,15 @@
         <v>37441</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C46" s="1">
         <v>7789</v>
@@ -3139,21 +3466,21 @@
         <v>45314</v>
       </c>
       <c r="I46" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J46" s="15">
         <v>35886</v>
       </c>
       <c r="K46" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1">
         <v>10942</v>
@@ -3168,7 +3495,7 @@
         <v>3</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H47" s="13">
         <v>45315</v>
@@ -3177,15 +3504,24 @@
         <v>38070</v>
       </c>
       <c r="K47" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="L47" t="s">
+        <v>119</v>
+      </c>
+      <c r="M47">
+        <v>35.72</v>
+      </c>
+      <c r="N47">
+        <v>95.58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C48" s="2">
         <v>6020</v>
@@ -3200,19 +3536,28 @@
         <v>4</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H48" s="13">
         <v>45317</v>
       </c>
       <c r="I48" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J48" s="15">
         <v>36284</v>
       </c>
       <c r="K48" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="L48" t="s">
+        <v>119</v>
+      </c>
+      <c r="M48">
+        <v>44.48</v>
+      </c>
+      <c r="N48">
+        <v>95.44</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
@@ -3220,7 +3565,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C49" s="2">
         <v>10038</v>
@@ -3241,13 +3586,13 @@
         <v>45317</v>
       </c>
       <c r="I49" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J49" s="15">
         <v>33386</v>
       </c>
       <c r="K49" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
@@ -3255,13 +3600,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C50" s="2">
         <v>6477</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -3279,7 +3624,7 @@
         <v>34470</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Participants' list and methods section, downloaded updated Participa list of the participants
</commit_message>
<xml_diff>
--- a/Experimental_scripts/Instructions_grids/REPSWITCH_List.xlsx
+++ b/Experimental_scripts/Instructions_grids/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\Experimental_scripts\Instructions_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D16206-49C2-4166-818C-16E08A984202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E5A52D-AF56-4FF3-BF43-295D02047070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="912" windowWidth="17736" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="125">
   <si>
     <t>Participant</t>
   </si>
@@ -518,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -558,11 +558,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1043,46 +1061,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:N3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:N3" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="A1:N3" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{D26CEDE0-6675-4478-AE1C-23ABA5C453CA}" name="NOMBRE" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{EFE7765A-783D-40C2-88ED-FBD03D4624CF}" name="ID" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{44B7B9A7-3620-4B2C-AA1F-A445ABB5A4AB}" name="CODE" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{53BF4CCF-E2C8-4075-828B-045D44DC2B5B}" name="DATE" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{D26CEDE0-6675-4478-AE1C-23ABA5C453CA}" name="NOMBRE" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{EFE7765A-783D-40C2-88ED-FBD03D4624CF}" name="ID" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{44B7B9A7-3620-4B2C-AA1F-A445ABB5A4AB}" name="CODE" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{53BF4CCF-E2C8-4075-828B-045D44DC2B5B}" name="DATE" dataDxfId="14"/>
     <tableColumn id="13" xr3:uid="{1015A516-CB69-4FC3-87A7-C4A13E267A67}" name="FechaNacimiento"/>
     <tableColumn id="14" xr3:uid="{EA8F05D9-3EE2-477E-9DA0-F765608E29F0}" name="Sexo"/>
-    <tableColumn id="6" xr3:uid="{1B290470-E23F-485F-AC08-FFFEAC9F056D}" name="VERSION" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{F0145F60-BB11-4B87-9FCD-BDAB0F3EDDB5}" name="LIST" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1B290470-E23F-485F-AC08-FFFEAC9F056D}" name="VERSION" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{F0145F60-BB11-4B87-9FCD-BDAB0F3EDDB5}" name="LIST" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:N50" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:N51" totalsRowCount="1">
   <autoFilter ref="A1:N50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
     <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID"/>
-    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="6" totalsRowDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0F7B8E20-170E-4530-BD6F-052C78EE98C3}" name="Version "/>
     <tableColumn id="3" xr3:uid="{C9573F81-3819-423D-82CC-5ABB8EA301BD}" name="List"/>
-    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="5" totalsRowDxfId="2"/>
     <tableColumn id="9" xr3:uid="{89FF1955-3050-4A09-8388-44DB3C7BAF8D}" name="Date"/>
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
     <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento"/>
-    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="4" totalsRowDxfId="1"/>
     <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador"/>
-    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed"/>
-    <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy"/>
+    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>AVERAGE(Table1[Type_speed])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy" totalsRowFunction="custom">
+      <totalsRowFormula>AVERAGE(Table1[Type_accuracy])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1543,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3062,6 +3084,15 @@
       <c r="K35" s="18" t="s">
         <v>85</v>
       </c>
+      <c r="L35" t="s">
+        <v>119</v>
+      </c>
+      <c r="M35">
+        <v>43.88</v>
+      </c>
+      <c r="N35">
+        <v>95.3</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
@@ -3094,6 +3125,15 @@
       <c r="K36" s="18" t="s">
         <v>85</v>
       </c>
+      <c r="L36" t="s">
+        <v>119</v>
+      </c>
+      <c r="M36">
+        <v>45.76</v>
+      </c>
+      <c r="N36">
+        <v>92.12</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
@@ -3296,6 +3336,15 @@
       <c r="K41" s="18" t="s">
         <v>85</v>
       </c>
+      <c r="L41" t="s">
+        <v>120</v>
+      </c>
+      <c r="M41">
+        <v>52.04</v>
+      </c>
+      <c r="N41">
+        <v>98.58</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -3372,6 +3421,15 @@
       <c r="K43" s="18" t="s">
         <v>84</v>
       </c>
+      <c r="L43" t="s">
+        <v>119</v>
+      </c>
+      <c r="M43">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="N43">
+        <v>94.42</v>
+      </c>
     </row>
     <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
@@ -3407,6 +3465,15 @@
       <c r="K44" s="18" t="s">
         <v>83</v>
       </c>
+      <c r="L44" t="s">
+        <v>120</v>
+      </c>
+      <c r="M44">
+        <v>41.4</v>
+      </c>
+      <c r="N44">
+        <v>90.52</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -3439,6 +3506,15 @@
       <c r="K45" s="18" t="s">
         <v>84</v>
       </c>
+      <c r="L45" t="s">
+        <v>119</v>
+      </c>
+      <c r="M45">
+        <v>41.8</v>
+      </c>
+      <c r="N45">
+        <v>98.06</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
@@ -3474,6 +3550,15 @@
       <c r="K46" s="18" t="s">
         <v>85</v>
       </c>
+      <c r="L46" t="s">
+        <v>120</v>
+      </c>
+      <c r="M46">
+        <v>51.2</v>
+      </c>
+      <c r="N46">
+        <v>97.62</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
@@ -3560,7 +3645,7 @@
         <v>95.44</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3594,8 +3679,17 @@
       <c r="K49" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49" t="s">
+        <v>120</v>
+      </c>
+      <c r="M49">
+        <v>61.56</v>
+      </c>
+      <c r="N49">
+        <v>95.84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3625,6 +3719,28 @@
       </c>
       <c r="K50" s="18" t="s">
         <v>83</v>
+      </c>
+      <c r="L50" t="s">
+        <v>120</v>
+      </c>
+      <c r="M50">
+        <v>45.46</v>
+      </c>
+      <c r="N50">
+        <v>97.52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="K51" s="22"/>
+      <c r="M51" s="23">
+        <f>AVERAGE(Table1[Type_speed])</f>
+        <v>42.137551020408168</v>
+      </c>
+      <c r="N51">
+        <f>AVERAGE(Table1[Type_accuracy])</f>
+        <v>93.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>